<commit_message>
fixed blip of dialtone when rotary dialing 1 first
</commit_message>
<xml_diff>
--- a/docs/ESP32 pin map.xlsx
+++ b/docs/ESP32 pin map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edge9\source\repos\Arduino Projects\RetroPhone\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4AC6E8-495B-4BCA-A56A-C3D1E4A9C508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9705C-839A-4627-B168-B8CC1F2A5D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17925" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{69EDDF2A-28D9-4AF5-8204-604043B8C710}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{69EDDF2A-28D9-4AF5-8204-604043B8C710}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
   <si>
     <t>GPIO</t>
   </si>
@@ -107,9 +107,6 @@
     <t>boot PWM</t>
   </si>
   <si>
-    <t>boot mode, onboard LED</t>
-  </si>
-  <si>
     <t>ADC</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>server/sender jumper</t>
   </si>
   <si>
-    <t>input only, no pullup/pulldown</t>
-  </si>
-  <si>
     <t>onboard 8MB SPI PSRAM</t>
   </si>
   <si>
@@ -450,13 +444,52 @@
   </si>
   <si>
     <t>Common Restrictions</t>
+  </si>
+  <si>
+    <t>pin has dedicated purpose and cannot be reassigned</t>
+  </si>
+  <si>
+    <t>available for use</t>
+  </si>
+  <si>
+    <t>strapping</t>
+  </si>
+  <si>
+    <t>strapping: must be low during boot</t>
+  </si>
+  <si>
+    <t>boot PWM, strapping low to enter flashing mode</t>
+  </si>
+  <si>
+    <t>Serial RX, strapping: high at boot</t>
+  </si>
+  <si>
+    <t>Serial TX, xmits debug logs at boot</t>
+  </si>
+  <si>
+    <t>boot PWM, strapping: must be high during boot</t>
+  </si>
+  <si>
+    <t>onboard LED, strapping: float/low enter flashing mode</t>
+  </si>
+  <si>
+    <t>input only, no internal pullup/pulldown</t>
+  </si>
+  <si>
+    <t>input only, internal no pullup/pulldown</t>
+  </si>
+  <si>
+    <t>pin has boot restrictions</t>
+  </si>
+  <si>
+    <t>pin not exposed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,14 +518,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +568,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -554,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -581,11 +614,16 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E06D21-DE31-4100-83D2-C57969AC0E34}">
-  <dimension ref="B1:N43"/>
+  <dimension ref="B1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24:T25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -937,7 +975,7 @@
     <col min="2" max="2" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
@@ -949,77 +987,77 @@
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.35">
       <c r="F1" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>113</v>
+      <c r="F2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="2:14" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>115</v>
+      <c r="C3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="K3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.35">
@@ -1029,13 +1067,13 @@
       <c r="C4" s="7"/>
       <c r="D4" s="10"/>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>9</v>
@@ -1049,10 +1087,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
@@ -1060,19 +1098,19 @@
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>9</v>
@@ -1086,10 +1124,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.35">
@@ -1098,17 +1136,19 @@
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>74</v>
+        <v>32</v>
+      </c>
+      <c r="N8" s="15" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
@@ -1117,19 +1157,19 @@
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="J9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>73</v>
+        <v>90</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
@@ -1221,23 +1261,25 @@
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
@@ -1245,20 +1287,20 @@
         <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.35">
@@ -1266,20 +1308,22 @@
         <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>120</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.35">
@@ -1288,22 +1332,22 @@
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
@@ -1311,10 +1355,10 @@
         <v>16</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -1323,10 +1367,10 @@
         <v>17</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="1"/>
     </row>
@@ -1336,14 +1380,14 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E22" s="1"/>
       <c r="J22" t="s">
-        <v>50</v>
-      </c>
-      <c r="N22" s="16" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="N22" s="15" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.35">
@@ -1352,14 +1396,14 @@
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E23" s="1"/>
       <c r="J23" t="s">
-        <v>51</v>
-      </c>
-      <c r="N23" s="16" t="s">
-        <v>71</v>
+        <v>50</v>
+      </c>
+      <c r="N23" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.35">
@@ -1368,24 +1412,24 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
-      <c r="E24" s="14"/>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>21</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E25" s="1"/>
       <c r="K25" t="s">
-        <v>107</v>
-      </c>
-      <c r="N25" s="16" t="s">
-        <v>70</v>
+        <v>105</v>
+      </c>
+      <c r="N25" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.35">
@@ -1394,17 +1438,17 @@
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E26" s="1"/>
       <c r="I26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K26" t="s">
-        <v>124</v>
-      </c>
-      <c r="N26" s="16" t="s">
-        <v>69</v>
+        <v>122</v>
+      </c>
+      <c r="N26" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.35">
@@ -1413,14 +1457,14 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="1"/>
       <c r="J27" t="s">
-        <v>52</v>
-      </c>
-      <c r="N27" s="16" t="s">
-        <v>68</v>
+        <v>51</v>
+      </c>
+      <c r="N27" s="15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.35">
@@ -1429,30 +1473,30 @@
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="14"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>25</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
-      </c>
-      <c r="N29" s="16" t="s">
-        <v>65</v>
+        <v>108</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.35">
@@ -1460,23 +1504,23 @@
         <v>26</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>31</v>
+        <v>21</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>30</v>
       </c>
       <c r="I30" t="s">
-        <v>111</v>
-      </c>
-      <c r="N30" s="16" t="s">
-        <v>66</v>
+        <v>109</v>
+      </c>
+      <c r="N30" s="15" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.35">
@@ -1484,20 +1528,20 @@
         <v>27</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H31" t="s">
-        <v>40</v>
-      </c>
-      <c r="N31" s="16" t="s">
-        <v>67</v>
+        <v>39</v>
+      </c>
+      <c r="N31" s="15" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.35">
@@ -1506,7 +1550,7 @@
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B33">
@@ -1514,7 +1558,7 @@
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
+      <c r="E33" s="13"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B34">
@@ -1522,7 +1566,7 @@
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="14"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B35">
@@ -1530,24 +1574,24 @@
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="14"/>
+      <c r="E35" s="13"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>32</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.35">
@@ -1555,17 +1599,17 @@
         <v>33</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.35">
@@ -1573,19 +1617,19 @@
         <v>34</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N38" s="16" t="s">
-        <v>63</v>
+        <v>26</v>
+      </c>
+      <c r="N38" s="15" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.35">
@@ -1593,19 +1637,19 @@
         <v>35</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N39" s="16" t="s">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="N39" s="15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.35">
@@ -1613,22 +1657,22 @@
         <v>36</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>90</v>
+        <v>86</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M40" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="N40" s="16" t="s">
-        <v>61</v>
+        <v>22</v>
+      </c>
+      <c r="M40" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N40" s="15" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.35">
@@ -1637,7 +1681,7 @@
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
-      <c r="E41" s="14"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B42">
@@ -1645,32 +1689,78 @@
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11"/>
-      <c r="E42" s="14"/>
+      <c r="E42" s="13"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>39</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E43" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M43" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="N43" s="16" t="s">
-        <v>62</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B45" s="11"/>
+      <c r="C45" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B46" s="5"/>
+      <c r="C46" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B47" s="7"/>
+      <c r="C47" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B48" s="12"/>
+      <c r="C48" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B49" s="1"/>
+      <c r="C49" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C49:E49"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated ESP32 pin map
</commit_message>
<xml_diff>
--- a/docs/ESP32 pin map.xlsx
+++ b/docs/ESP32 pin map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edge9\source\repos\Arduino Projects\RetroPhone\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F9705C-839A-4627-B168-B8CC1F2A5D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305F33B7-F592-4B5B-91A9-0B3FCEDF2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{69EDDF2A-28D9-4AF5-8204-604043B8C710}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="138">
   <si>
     <t>GPIO</t>
   </si>
@@ -483,13 +483,16 @@
   </si>
   <si>
     <t>pin not exposed</t>
+  </si>
+  <si>
+    <t>REF: strapping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,6 +517,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -584,10 +595,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -624,8 +636,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -966,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E06D21-DE31-4100-83D2-C57969AC0E34}">
   <dimension ref="B1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46:E46"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,6 +1005,9 @@
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E2" s="18" t="s">
+        <v>137</v>
+      </c>
       <c r="F2" s="14" t="s">
         <v>111</v>
       </c>
@@ -1762,8 +1779,11 @@
     <mergeCell ref="C49:E49"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{8E5CD4BE-B80F-4843-BBC9-8C3F58BC7F67}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved some pins around to get off ADC2 now that we are using wifi, which uses ADC2
</commit_message>
<xml_diff>
--- a/docs/ESP32 pin map.xlsx
+++ b/docs/ESP32 pin map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edge9\source\repos\Arduino Projects\RetroPhone\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305F33B7-F592-4B5B-91A9-0B3FCEDF2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB93913-F658-459B-874C-B4D1045BB5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="17860" xr2:uid="{69EDDF2A-28D9-4AF5-8204-604043B8C710}"/>
+    <workbookView xWindow="20475" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{69EDDF2A-28D9-4AF5-8204-604043B8C710}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <author>tc={D4611B6D-5F55-4481-B991-8A2CE5B0115D}</author>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{1EFACA59-C815-442D-A8A2-DC592F52C9B2}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{1EFACA59-C815-442D-A8A2-DC592F52C9B2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,7 +51,7 @@
     Supports two SPI busses on any pins.</t>
       </text>
     </comment>
-    <comment ref="K2" authorId="1" shapeId="0" xr:uid="{594B4F03-7E6C-4731-8829-FA058E504210}">
+    <comment ref="L2" authorId="1" shapeId="0" xr:uid="{594B4F03-7E6C-4731-8829-FA058E504210}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -479,13 +479,13 @@
     <t>input only, internal no pullup/pulldown</t>
   </si>
   <si>
-    <t>pin has boot restrictions</t>
-  </si>
-  <si>
     <t>pin not exposed</t>
   </si>
   <si>
     <t>REF: strapping</t>
+  </si>
+  <si>
+    <t>pin has boot and/or wifi restrictions</t>
   </si>
 </sst>
 </file>
@@ -633,10 +633,10 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -964,10 +964,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J2" dT="2023-08-04T03:47:17.75" personId="{763C87D4-9ECF-4D67-B01F-5FDD4C083499}" id="{1EFACA59-C815-442D-A8A2-DC592F52C9B2}">
+  <threadedComment ref="K2" dT="2023-08-04T03:47:17.75" personId="{763C87D4-9ECF-4D67-B01F-5FDD4C083499}" id="{1EFACA59-C815-442D-A8A2-DC592F52C9B2}">
     <text>Supports two SPI busses on any pins.</text>
   </threadedComment>
-  <threadedComment ref="K2" dT="2023-08-04T03:48:22.60" personId="{763C87D4-9ECF-4D67-B01F-5FDD4C083499}" id="{594B4F03-7E6C-4731-8829-FA058E504210}">
+  <threadedComment ref="L2" dT="2023-08-04T03:48:22.60" personId="{763C87D4-9ECF-4D67-B01F-5FDD4C083499}" id="{594B4F03-7E6C-4731-8829-FA058E504210}">
     <text>Supports two I2C busses on any pins.</text>
   </threadedComment>
   <threadedComment ref="N3" dT="2023-08-04T03:44:57.91" personId="{763C87D4-9ECF-4D67-B01F-5FDD4C083499}" id="{D4611B6D-5F55-4481-B991-8A2CE5B0115D}">
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E06D21-DE31-4100-83D2-C57969AC0E34}">
   <dimension ref="B1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,23 +990,23 @@
     <col min="3" max="3" width="29.1796875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="9.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="E2" s="18" t="s">
-        <v>137</v>
+      <c r="E2" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F2" s="14" t="s">
         <v>111</v>
@@ -1017,8 +1017,8 @@
       <c r="H2" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>106</v>
+      <c r="I2" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>106</v>
@@ -1026,8 +1026,8 @@
       <c r="K2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>111</v>
+      <c r="L2" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="M2" s="14" t="s">
         <v>111</v>
@@ -1050,25 +1050,25 @@
         <v>123</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>56</v>
@@ -1087,13 +1087,13 @@
         <v>128</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>34</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
@@ -1124,13 +1124,13 @@
         <v>132</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>33</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.35">
@@ -1158,10 +1158,10 @@
       <c r="E8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>32</v>
       </c>
       <c r="N8" s="15" t="s">
@@ -1179,11 +1179,11 @@
       <c r="E9" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="J9" t="s">
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="K9" t="s">
         <v>48</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="N9" s="15" t="s">
         <v>72</v>
@@ -1287,16 +1287,16 @@
         <v>127</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>37</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>44</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
@@ -1310,13 +1310,13 @@
         <v>121</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>36</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1324,22 +1324,20 @@
       <c r="B18">
         <v>14</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="9" t="s">
         <v>120</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>38</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1355,16 +1353,16 @@
         <v>131</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>35</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>47</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.35">
@@ -1400,7 +1398,7 @@
         <v>81</v>
       </c>
       <c r="E22" s="1"/>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>49</v>
       </c>
       <c r="N22" s="15" t="s">
@@ -1416,7 +1414,7 @@
         <v>82</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>50</v>
       </c>
       <c r="N23" s="15" t="s">
@@ -1442,7 +1440,7 @@
         <v>119</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>105</v>
       </c>
       <c r="N25" s="15" t="s">
@@ -1453,15 +1451,17 @@
       <c r="B26">
         <v>22</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D26" s="9" t="s">
         <v>118</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>107</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>122</v>
       </c>
       <c r="N26" s="15" t="s">
@@ -1472,12 +1472,14 @@
       <c r="B27">
         <v>23</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="D27" s="9" t="s">
         <v>84</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>51</v>
       </c>
       <c r="N27" s="15" t="s">
@@ -1503,13 +1505,13 @@
         <v>116</v>
       </c>
       <c r="E29" s="1"/>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="H29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>108</v>
       </c>
       <c r="N29" s="15" t="s">
@@ -1527,13 +1529,13 @@
         <v>117</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="H30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>109</v>
       </c>
       <c r="N30" s="15" t="s">
@@ -1551,10 +1553,10 @@
         <v>85</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>39</v>
       </c>
       <c r="N31" s="15" t="s">
@@ -1598,16 +1600,16 @@
         <v>32</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>87</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1615,17 +1617,15 @@
       <c r="B37">
         <v>33</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>95</v>
-      </c>
+      <c r="C37" s="1"/>
       <c r="D37" s="9" t="s">
         <v>79</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       <c r="E38" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>26</v>
       </c>
       <c r="N38" s="15" t="s">
@@ -1662,7 +1662,7 @@
       <c r="E39" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>27</v>
       </c>
       <c r="N39" s="15" t="s">
@@ -1682,7 +1682,7 @@
       <c r="E40" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M40" s="12" t="s">
@@ -1721,7 +1721,7 @@
       <c r="E43" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M43" s="12" t="s">
@@ -1733,43 +1733,43 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B45" s="11"/>
-      <c r="C45" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
+      <c r="C45" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B46" s="5"/>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B47" s="7"/>
-      <c r="C47" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
+      <c r="C47" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B48" s="12"/>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" s="1"/>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="16"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>